<commit_message>
fixed matsmo_score_ changed type from integer to decimal
</commit_message>
<xml_diff>
--- a/dictionaries/outcome/1_7/1_7_yearly_rep.xlsx
+++ b/dictionaries/outcome/1_7/1_7_yearly_rep.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demetrisavraam/Desktop/GitHub/ds-dictionaries/dictionaries/outcome/1_7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\ATHLETE\HARMO\git_hub\ds-dictionaries\dictionaries\outcome\1_7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA2AA96-F00B-AA4B-9ACA-190F2A91DF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187B821C-E1BA-4B89-975C-CDB8D6A3D46F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -1350,7 +1350,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1410,12 +1410,18 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -1488,7 +1494,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1526,6 +1532,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1993,19 +2000,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG159"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140:XFD159"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A130" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="15.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="97.83203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="29.140625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="15.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="97.85546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:59" ht="15" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2074,7 +2081,7 @@
       <c r="BF1"/>
       <c r="BG1"/>
     </row>
-    <row r="2" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:59" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2088,7 +2095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2100,7 +2107,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:59" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
@@ -2114,7 +2121,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" ht="15" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -2129,7 +2136,7 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" ht="15" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -2144,7 +2151,7 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" ht="15" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>356</v>
       </c>
@@ -2159,7 +2166,7 @@
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" ht="15" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>358</v>
       </c>
@@ -2174,7 +2181,7 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:59" ht="15" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -2189,7 +2196,7 @@
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:59" ht="15" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -2204,7 +2211,7 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:59" ht="15" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -2219,7 +2226,7 @@
       </c>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:59" ht="15" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -2234,7 +2241,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:59" ht="15" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>38</v>
       </c>
@@ -2248,7 +2255,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:59" ht="15" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>40</v>
       </c>
@@ -2262,7 +2269,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:59" ht="15" customHeight="1">
       <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
@@ -2276,7 +2283,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:59" ht="15" customHeight="1">
       <c r="A16" s="4" t="s">
         <v>44</v>
       </c>
@@ -2290,7 +2297,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15" customHeight="1">
       <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
@@ -2304,7 +2311,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15" customHeight="1">
       <c r="A18" s="4" t="s">
         <v>48</v>
       </c>
@@ -2318,7 +2325,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15" customHeight="1">
       <c r="A19" s="4" t="s">
         <v>50</v>
       </c>
@@ -2332,7 +2339,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15" customHeight="1">
       <c r="A20" s="4" t="s">
         <v>52</v>
       </c>
@@ -2346,7 +2353,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15" customHeight="1">
       <c r="A21" s="17" t="s">
         <v>354</v>
       </c>
@@ -2360,7 +2367,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15" customHeight="1">
       <c r="A22" s="4" t="s">
         <v>54</v>
       </c>
@@ -2374,7 +2381,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="15" customHeight="1">
       <c r="A23" s="4" t="s">
         <v>56</v>
       </c>
@@ -2388,7 +2395,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="15" customHeight="1">
       <c r="A24" s="4" t="s">
         <v>58</v>
       </c>
@@ -2402,7 +2409,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="15" customHeight="1">
       <c r="A25" s="4" t="s">
         <v>60</v>
       </c>
@@ -2416,7 +2423,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="15" customHeight="1">
       <c r="A26" s="4" t="s">
         <v>62</v>
       </c>
@@ -2430,7 +2437,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="15" customHeight="1">
       <c r="A27" s="4" t="s">
         <v>64</v>
       </c>
@@ -2444,7 +2451,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15" customHeight="1">
       <c r="A28" s="4" t="s">
         <v>66</v>
       </c>
@@ -2458,7 +2465,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="15" customHeight="1">
       <c r="A29" s="4" t="s">
         <v>68</v>
       </c>
@@ -2472,7 +2479,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="15" customHeight="1">
       <c r="A30" s="9" t="s">
         <v>71</v>
       </c>
@@ -2486,7 +2493,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15" customHeight="1">
       <c r="A31" s="9" t="s">
         <v>73</v>
       </c>
@@ -2500,7 +2507,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="15" customHeight="1">
       <c r="A32" s="9" t="s">
         <v>74</v>
       </c>
@@ -2514,7 +2521,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="15" customHeight="1">
       <c r="A33" s="9" t="s">
         <v>76</v>
       </c>
@@ -2528,7 +2535,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="15" customHeight="1">
       <c r="A34" s="9" t="s">
         <v>78</v>
       </c>
@@ -2542,7 +2549,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="15" customHeight="1">
       <c r="A35" s="9" t="s">
         <v>80</v>
       </c>
@@ -2556,7 +2563,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="15" customHeight="1">
       <c r="A36" s="4" t="s">
         <v>82</v>
       </c>
@@ -2570,7 +2577,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="15" customHeight="1">
       <c r="A37" s="9" t="s">
         <v>84</v>
       </c>
@@ -2584,7 +2591,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="15" customHeight="1">
       <c r="A38" s="9" t="s">
         <v>86</v>
       </c>
@@ -2598,7 +2605,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="15" customHeight="1">
       <c r="A39" s="9" t="s">
         <v>89</v>
       </c>
@@ -2612,7 +2619,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="15" customHeight="1">
       <c r="A40" s="9" t="s">
         <v>91</v>
       </c>
@@ -2626,7 +2633,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="15" customHeight="1">
       <c r="A41" s="9" t="s">
         <v>93</v>
       </c>
@@ -2640,7 +2647,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="15" customHeight="1">
       <c r="A42" s="9" t="s">
         <v>95</v>
       </c>
@@ -2654,7 +2661,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="15" customHeight="1">
       <c r="A43" s="9" t="s">
         <v>97</v>
       </c>
@@ -2668,7 +2675,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="15" customHeight="1">
       <c r="A44" s="9" t="s">
         <v>99</v>
       </c>
@@ -2682,7 +2689,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="15" customHeight="1">
       <c r="A45" s="9" t="s">
         <v>101</v>
       </c>
@@ -2696,7 +2703,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="15" customHeight="1">
       <c r="A46" s="9" t="s">
         <v>103</v>
       </c>
@@ -2710,7 +2717,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="15" customHeight="1">
       <c r="A47" s="9" t="s">
         <v>105</v>
       </c>
@@ -2724,7 +2731,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="15" customHeight="1">
       <c r="A48" s="9" t="s">
         <v>107</v>
       </c>
@@ -2738,7 +2745,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="15" customHeight="1">
       <c r="A49" s="9" t="s">
         <v>109</v>
       </c>
@@ -2752,7 +2759,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="15" customHeight="1">
       <c r="A50" s="9" t="s">
         <v>111</v>
       </c>
@@ -2766,7 +2773,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="15" customHeight="1">
       <c r="A51" s="9" t="s">
         <v>113</v>
       </c>
@@ -2780,7 +2787,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="15" customHeight="1">
       <c r="A52" s="9" t="s">
         <v>115</v>
       </c>
@@ -2794,7 +2801,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="15" customHeight="1">
       <c r="A53" s="9" t="s">
         <v>117</v>
       </c>
@@ -2808,7 +2815,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="15" customHeight="1">
       <c r="A54" s="9" t="s">
         <v>119</v>
       </c>
@@ -2822,7 +2829,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="15" customHeight="1">
       <c r="A55" s="9" t="s">
         <v>121</v>
       </c>
@@ -2836,7 +2843,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="15" customHeight="1">
       <c r="A56" s="9" t="s">
         <v>123</v>
       </c>
@@ -2850,7 +2857,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="15" customHeight="1">
       <c r="A57" s="9" t="s">
         <v>125</v>
       </c>
@@ -2864,7 +2871,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="15" customHeight="1">
       <c r="A58" s="9" t="s">
         <v>127</v>
       </c>
@@ -2878,7 +2885,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="15" customHeight="1">
       <c r="A59" s="9" t="s">
         <v>129</v>
       </c>
@@ -2892,7 +2899,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="15" customHeight="1">
       <c r="A60" s="9" t="s">
         <v>131</v>
       </c>
@@ -2906,7 +2913,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="15" customHeight="1">
       <c r="A61" s="9" t="s">
         <v>133</v>
       </c>
@@ -2920,7 +2927,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="15" customHeight="1">
       <c r="A62" s="9" t="s">
         <v>135</v>
       </c>
@@ -2934,7 +2941,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="15" customHeight="1">
       <c r="A63" s="9" t="s">
         <v>137</v>
       </c>
@@ -2948,7 +2955,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="15" customHeight="1">
       <c r="A64" s="9" t="s">
         <v>139</v>
       </c>
@@ -2962,7 +2969,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="15" customHeight="1">
       <c r="A65" s="9" t="s">
         <v>141</v>
       </c>
@@ -2976,7 +2983,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="15" customHeight="1">
       <c r="A66" s="9" t="s">
         <v>143</v>
       </c>
@@ -2990,7 +2997,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="15" customHeight="1">
       <c r="A67" s="9" t="s">
         <v>145</v>
       </c>
@@ -3004,7 +3011,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="15" customHeight="1">
       <c r="A68" s="9" t="s">
         <v>147</v>
       </c>
@@ -3018,7 +3025,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="15" customHeight="1">
       <c r="A69" s="9" t="s">
         <v>149</v>
       </c>
@@ -3032,7 +3039,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="15" customHeight="1">
       <c r="A70" s="9" t="s">
         <v>151</v>
       </c>
@@ -3046,7 +3053,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="15" customHeight="1">
       <c r="A71" s="9" t="s">
         <v>153</v>
       </c>
@@ -3060,7 +3067,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="15" customHeight="1">
       <c r="A72" s="9" t="s">
         <v>155</v>
       </c>
@@ -3074,7 +3081,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="15" customHeight="1">
       <c r="A73" s="9" t="s">
         <v>157</v>
       </c>
@@ -3088,7 +3095,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="15" customHeight="1">
       <c r="A74" s="9" t="s">
         <v>159</v>
       </c>
@@ -3102,7 +3109,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" ht="15" customHeight="1">
       <c r="A75" s="9" t="s">
         <v>161</v>
       </c>
@@ -3116,7 +3123,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" ht="15" customHeight="1">
       <c r="A76" s="9" t="s">
         <v>163</v>
       </c>
@@ -3130,7 +3137,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" ht="15" customHeight="1">
       <c r="A77" s="9" t="s">
         <v>165</v>
       </c>
@@ -3144,7 +3151,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="15" customHeight="1">
       <c r="A78" s="9" t="s">
         <v>167</v>
       </c>
@@ -3158,7 +3165,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" ht="15" customHeight="1">
       <c r="A79" s="9" t="s">
         <v>169</v>
       </c>
@@ -3172,7 +3179,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" ht="15" customHeight="1">
       <c r="A80" s="9" t="s">
         <v>171</v>
       </c>
@@ -3186,7 +3193,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" ht="15" customHeight="1">
       <c r="A81" s="9" t="s">
         <v>173</v>
       </c>
@@ -3200,7 +3207,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="15" customHeight="1">
       <c r="A82" s="9" t="s">
         <v>175</v>
       </c>
@@ -3214,7 +3221,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="15" customHeight="1">
       <c r="A83" s="9" t="s">
         <v>177</v>
       </c>
@@ -3228,7 +3235,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" ht="15" customHeight="1">
       <c r="A84" s="9" t="s">
         <v>179</v>
       </c>
@@ -3242,7 +3249,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" ht="15" customHeight="1">
       <c r="A85" s="9" t="s">
         <v>181</v>
       </c>
@@ -3256,7 +3263,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" ht="15" customHeight="1">
       <c r="A86" s="9" t="s">
         <v>183</v>
       </c>
@@ -3270,7 +3277,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" ht="15" customHeight="1">
       <c r="A87" s="9" t="s">
         <v>185</v>
       </c>
@@ -3284,7 +3291,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" ht="15" customHeight="1">
       <c r="A88" s="9" t="s">
         <v>187</v>
       </c>
@@ -3298,7 +3305,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" ht="15" customHeight="1">
       <c r="A89" s="9" t="s">
         <v>189</v>
       </c>
@@ -3312,7 +3319,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" ht="15" customHeight="1">
       <c r="A90" s="9" t="s">
         <v>191</v>
       </c>
@@ -3326,7 +3333,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" ht="15" customHeight="1">
       <c r="A91" s="9" t="s">
         <v>193</v>
       </c>
@@ -3340,7 +3347,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" ht="15" customHeight="1">
       <c r="A92" s="9" t="s">
         <v>195</v>
       </c>
@@ -3354,7 +3361,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" ht="15" customHeight="1">
       <c r="A93" s="9" t="s">
         <v>197</v>
       </c>
@@ -3368,7 +3375,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" ht="15" customHeight="1">
       <c r="A94" s="9" t="s">
         <v>199</v>
       </c>
@@ -3382,7 +3389,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" ht="15" customHeight="1">
       <c r="A95" s="9" t="s">
         <v>201</v>
       </c>
@@ -3396,7 +3403,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" ht="15" customHeight="1">
       <c r="A96" s="9" t="s">
         <v>203</v>
       </c>
@@ -3410,7 +3417,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" ht="15" customHeight="1">
       <c r="A97" s="9" t="s">
         <v>205</v>
       </c>
@@ -3424,7 +3431,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" ht="15" customHeight="1">
       <c r="A98" s="9" t="s">
         <v>207</v>
       </c>
@@ -3438,7 +3445,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="15" customHeight="1">
       <c r="A99" s="9" t="s">
         <v>209</v>
       </c>
@@ -3452,7 +3459,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" ht="15" customHeight="1">
       <c r="A100" s="9" t="s">
         <v>211</v>
       </c>
@@ -3466,7 +3473,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" ht="15" customHeight="1">
       <c r="A101" s="9" t="s">
         <v>213</v>
       </c>
@@ -3480,7 +3487,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" ht="15" customHeight="1">
       <c r="A102" s="9" t="s">
         <v>215</v>
       </c>
@@ -3494,7 +3501,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" ht="15" customHeight="1">
       <c r="A103" s="9" t="s">
         <v>217</v>
       </c>
@@ -3508,7 +3515,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" ht="15" customHeight="1">
       <c r="A104" s="9" t="s">
         <v>219</v>
       </c>
@@ -3522,7 +3529,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" ht="15" customHeight="1">
       <c r="A105" s="9" t="s">
         <v>221</v>
       </c>
@@ -3536,7 +3543,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" ht="15" customHeight="1">
       <c r="A106" s="9" t="s">
         <v>223</v>
       </c>
@@ -3550,7 +3557,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" ht="15" customHeight="1">
       <c r="A107" s="9" t="s">
         <v>225</v>
       </c>
@@ -3564,7 +3571,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" ht="15" customHeight="1">
       <c r="A108" s="9" t="s">
         <v>227</v>
       </c>
@@ -3578,7 +3585,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" ht="15" customHeight="1">
       <c r="A109" s="9" t="s">
         <v>229</v>
       </c>
@@ -3592,7 +3599,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" ht="15" customHeight="1">
       <c r="A110" s="11" t="s">
         <v>231</v>
       </c>
@@ -3606,7 +3613,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" ht="15" customHeight="1">
       <c r="A111" t="s">
         <v>303</v>
       </c>
@@ -3620,7 +3627,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" ht="15" customHeight="1">
       <c r="A112" t="s">
         <v>305</v>
       </c>
@@ -3634,7 +3641,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" ht="15" customHeight="1">
       <c r="A113" s="16" t="s">
         <v>349</v>
       </c>
@@ -3648,7 +3655,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" ht="15" customHeight="1">
       <c r="A114" t="s">
         <v>309</v>
       </c>
@@ -3662,7 +3669,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="15" customHeight="1">
       <c r="A115" t="s">
         <v>350</v>
       </c>
@@ -3676,7 +3683,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" ht="15" customHeight="1">
       <c r="A116" t="s">
         <v>351</v>
       </c>
@@ -3690,7 +3697,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" ht="15" customHeight="1">
       <c r="A117" t="s">
         <v>315</v>
       </c>
@@ -3704,7 +3711,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" ht="15" customHeight="1">
       <c r="A118" t="s">
         <v>352</v>
       </c>
@@ -3718,7 +3725,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" ht="15" customHeight="1">
       <c r="A119" t="s">
         <v>353</v>
       </c>
@@ -3732,7 +3739,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" ht="15" customHeight="1">
       <c r="A120" t="s">
         <v>321</v>
       </c>
@@ -3746,7 +3753,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" ht="15" customHeight="1">
       <c r="A121" t="s">
         <v>323</v>
       </c>
@@ -3760,7 +3767,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" ht="15" customHeight="1">
       <c r="A122" t="s">
         <v>325</v>
       </c>
@@ -3774,7 +3781,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" ht="15" customHeight="1">
       <c r="A123" t="s">
         <v>327</v>
       </c>
@@ -3788,7 +3795,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" ht="15" customHeight="1">
       <c r="A124" t="s">
         <v>329</v>
       </c>
@@ -3802,7 +3809,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" ht="15" customHeight="1">
       <c r="A125" t="s">
         <v>366</v>
       </c>
@@ -3816,7 +3823,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" ht="15" customHeight="1">
       <c r="A126" s="20" t="s">
         <v>365</v>
       </c>
@@ -3830,7 +3837,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" ht="15" customHeight="1">
       <c r="A127" t="s">
         <v>364</v>
       </c>
@@ -3844,7 +3851,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" ht="15" customHeight="1">
       <c r="A128" t="s">
         <v>363</v>
       </c>
@@ -3858,7 +3865,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" ht="15" customHeight="1">
       <c r="A129" s="20" t="s">
         <v>367</v>
       </c>
@@ -3872,7 +3879,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" ht="15" customHeight="1">
       <c r="A130" t="s">
         <v>362</v>
       </c>
@@ -3886,7 +3893,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" ht="15" customHeight="1">
       <c r="A131" s="20" t="s">
         <v>361</v>
       </c>
@@ -3900,7 +3907,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" ht="15" customHeight="1">
       <c r="A132" s="20" t="s">
         <v>368</v>
       </c>
@@ -3914,7 +3921,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" ht="15" customHeight="1">
       <c r="A133" t="s">
         <v>360</v>
       </c>
@@ -3928,12 +3935,12 @@
         <v>348</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" ht="15" customHeight="1">
       <c r="A134" t="s">
         <v>393</v>
       </c>
-      <c r="B134" t="s">
-        <v>5</v>
+      <c r="B134" s="27" t="s">
+        <v>12</v>
       </c>
       <c r="C134" t="s">
         <v>12</v>
@@ -3942,7 +3949,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" ht="15" customHeight="1">
       <c r="A135" t="s">
         <v>374</v>
       </c>
@@ -3956,7 +3963,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" ht="15" customHeight="1">
       <c r="A136" t="s">
         <v>394</v>
       </c>
@@ -3970,7 +3977,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" ht="15" customHeight="1">
       <c r="A137" t="s">
         <v>377</v>
       </c>
@@ -3984,7 +3991,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" ht="15" customHeight="1">
       <c r="A138" t="s">
         <v>381</v>
       </c>
@@ -3998,7 +4005,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" ht="15" customHeight="1">
       <c r="A139" s="23" t="s">
         <v>391</v>
       </c>
@@ -4012,7 +4019,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="140" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A140" s="24" t="s">
         <v>395</v>
       </c>
@@ -4026,7 +4033,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="141" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A141" s="24" t="s">
         <v>397</v>
       </c>
@@ -4040,7 +4047,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="142" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A142" s="24" t="s">
         <v>399</v>
       </c>
@@ -4054,7 +4061,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="143" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A143" s="24" t="s">
         <v>401</v>
       </c>
@@ -4068,7 +4075,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="144" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A144" s="24" t="s">
         <v>403</v>
       </c>
@@ -4082,7 +4089,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="145" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A145" s="24" t="s">
         <v>405</v>
       </c>
@@ -4096,7 +4103,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="146" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A146" s="24" t="s">
         <v>407</v>
       </c>
@@ -4110,7 +4117,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="147" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A147" s="24" t="s">
         <v>409</v>
       </c>
@@ -4124,7 +4131,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="148" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A148" s="24" t="s">
         <v>411</v>
       </c>
@@ -4138,7 +4145,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="149" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A149" s="24" t="s">
         <v>413</v>
       </c>
@@ -4152,7 +4159,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="150" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A150" s="24" t="s">
         <v>415</v>
       </c>
@@ -4166,7 +4173,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="151" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A151" s="24" t="s">
         <v>417</v>
       </c>
@@ -4180,7 +4187,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="152" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A152" s="24" t="s">
         <v>419</v>
       </c>
@@ -4194,7 +4201,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="153" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A153" s="24" t="s">
         <v>421</v>
       </c>
@@ -4208,7 +4215,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="154" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A154" s="24" t="s">
         <v>423</v>
       </c>
@@ -4222,7 +4229,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="155" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A155" s="24" t="s">
         <v>425</v>
       </c>
@@ -4236,7 +4243,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="156" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A156" s="24" t="s">
         <v>427</v>
       </c>
@@ -4250,7 +4257,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="157" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A157" s="24" t="s">
         <v>429</v>
       </c>
@@ -4264,7 +4271,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="158" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A158" s="24" t="s">
         <v>431</v>
       </c>
@@ -4278,7 +4285,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="159" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A159" s="24" t="s">
         <v>433</v>
       </c>
@@ -4310,14 +4317,14 @@
       <selection activeCell="D238" sqref="D238"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" style="1" customWidth="1"/>
-    <col min="2" max="4" width="18.5" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="37.28515625" style="1" customWidth="1"/>
+    <col min="2" max="4" width="18.42578125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -4331,7 +4338,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -4345,7 +4352,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -4359,7 +4366,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -4373,7 +4380,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -4387,7 +4394,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -4401,7 +4408,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -4415,7 +4422,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
@@ -4429,7 +4436,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -4443,7 +4450,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="15" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -4457,7 +4464,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="15" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
@@ -4471,7 +4478,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -4485,7 +4492,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15" customHeight="1">
       <c r="A13" s="20" t="s">
         <v>356</v>
       </c>
@@ -4499,7 +4506,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="15" customHeight="1">
       <c r="A14" s="20" t="s">
         <v>356</v>
       </c>
@@ -4513,7 +4520,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="15" customHeight="1">
       <c r="A15" s="20" t="s">
         <v>358</v>
       </c>
@@ -4527,7 +4534,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15" customHeight="1">
       <c r="A16" s="20" t="s">
         <v>358</v>
       </c>
@@ -4541,7 +4548,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>34</v>
       </c>
@@ -4555,7 +4562,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>34</v>
       </c>
@@ -4569,7 +4576,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15" customHeight="1">
       <c r="A19" s="5" t="s">
         <v>36</v>
       </c>
@@ -4583,7 +4590,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>36</v>
       </c>
@@ -4597,7 +4604,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15" customHeight="1">
       <c r="A21" s="4" t="s">
         <v>54</v>
       </c>
@@ -4611,7 +4618,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15" customHeight="1">
       <c r="A22" s="4" t="s">
         <v>54</v>
       </c>
@@ -4625,7 +4632,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="15" customHeight="1">
       <c r="A23" s="4" t="s">
         <v>56</v>
       </c>
@@ -4639,7 +4646,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="15" customHeight="1">
       <c r="A24" s="4" t="s">
         <v>56</v>
       </c>
@@ -4653,7 +4660,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="15" customHeight="1">
       <c r="A25" s="4" t="s">
         <v>60</v>
       </c>
@@ -4667,7 +4674,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="15" customHeight="1">
       <c r="A26" s="4" t="s">
         <v>60</v>
       </c>
@@ -4681,7 +4688,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="15" customHeight="1">
       <c r="A27" s="4" t="s">
         <v>62</v>
       </c>
@@ -4695,7 +4702,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15" customHeight="1">
       <c r="A28" s="4" t="s">
         <v>62</v>
       </c>
@@ -4709,7 +4716,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="15" customHeight="1">
       <c r="A29" s="4" t="s">
         <v>64</v>
       </c>
@@ -4723,7 +4730,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="15" customHeight="1">
       <c r="A30" s="4" t="s">
         <v>64</v>
       </c>
@@ -4737,7 +4744,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15" customHeight="1">
       <c r="A31" s="4" t="s">
         <v>66</v>
       </c>
@@ -4751,7 +4758,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="15" customHeight="1">
       <c r="A32" s="4" t="s">
         <v>66</v>
       </c>
@@ -4765,7 +4772,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="15" customHeight="1">
       <c r="A33" s="4" t="s">
         <v>68</v>
       </c>
@@ -4779,7 +4786,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="15" customHeight="1">
       <c r="A34" s="4" t="s">
         <v>68</v>
       </c>
@@ -4793,7 +4800,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="15" customHeight="1">
       <c r="A35" s="4" t="s">
         <v>91</v>
       </c>
@@ -4807,7 +4814,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="15" customHeight="1">
       <c r="A36" s="4" t="s">
         <v>91</v>
       </c>
@@ -4821,7 +4828,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="15" customHeight="1">
       <c r="A37" s="4" t="s">
         <v>91</v>
       </c>
@@ -4835,7 +4842,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="15" customHeight="1">
       <c r="A38" s="4" t="s">
         <v>91</v>
       </c>
@@ -4849,7 +4856,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="15" customHeight="1">
       <c r="A39" s="4" t="s">
         <v>91</v>
       </c>
@@ -4863,7 +4870,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="15" customHeight="1">
       <c r="A40" s="4" t="s">
         <v>91</v>
       </c>
@@ -4877,7 +4884,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="15" customHeight="1">
       <c r="A41" s="4" t="s">
         <v>89</v>
       </c>
@@ -4891,7 +4898,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="15" customHeight="1">
       <c r="A42" s="4" t="s">
         <v>89</v>
       </c>
@@ -4905,7 +4912,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="15" customHeight="1">
       <c r="A43" s="4" t="s">
         <v>89</v>
       </c>
@@ -4919,7 +4926,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="15" customHeight="1">
       <c r="A44" s="4" t="s">
         <v>89</v>
       </c>
@@ -4933,7 +4940,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="15" customHeight="1">
       <c r="A45" s="4" t="s">
         <v>89</v>
       </c>
@@ -4947,7 +4954,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="15" customHeight="1">
       <c r="A46" s="4" t="s">
         <v>89</v>
       </c>
@@ -4961,7 +4968,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="15" customHeight="1">
       <c r="A47" s="4" t="s">
         <v>105</v>
       </c>
@@ -4975,7 +4982,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="15" customHeight="1">
       <c r="A48" s="4" t="s">
         <v>105</v>
       </c>
@@ -4989,7 +4996,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="15" customHeight="1">
       <c r="A49" s="4" t="s">
         <v>105</v>
       </c>
@@ -5003,7 +5010,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="15" customHeight="1">
       <c r="A50" s="4" t="s">
         <v>105</v>
       </c>
@@ -5017,7 +5024,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="15" customHeight="1">
       <c r="A51" s="4" t="s">
         <v>105</v>
       </c>
@@ -5031,7 +5038,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="15" customHeight="1">
       <c r="A52" s="4" t="s">
         <v>105</v>
       </c>
@@ -5045,7 +5052,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="15" customHeight="1">
       <c r="A53" s="4" t="s">
         <v>103</v>
       </c>
@@ -5059,7 +5066,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="15" customHeight="1">
       <c r="A54" s="4" t="s">
         <v>103</v>
       </c>
@@ -5073,7 +5080,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="15" customHeight="1">
       <c r="A55" s="4" t="s">
         <v>103</v>
       </c>
@@ -5087,7 +5094,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="15" customHeight="1">
       <c r="A56" s="4" t="s">
         <v>103</v>
       </c>
@@ -5101,7 +5108,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="15" customHeight="1">
       <c r="A57" s="4" t="s">
         <v>103</v>
       </c>
@@ -5115,7 +5122,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="15" customHeight="1">
       <c r="A58" s="4" t="s">
         <v>103</v>
       </c>
@@ -5129,7 +5136,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="15" customHeight="1">
       <c r="A59" s="4" t="s">
         <v>119</v>
       </c>
@@ -5143,7 +5150,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="15" customHeight="1">
       <c r="A60" s="4" t="s">
         <v>119</v>
       </c>
@@ -5157,7 +5164,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="15" customHeight="1">
       <c r="A61" s="4" t="s">
         <v>119</v>
       </c>
@@ -5171,7 +5178,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="15" customHeight="1">
       <c r="A62" s="4" t="s">
         <v>119</v>
       </c>
@@ -5185,7 +5192,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="15" customHeight="1">
       <c r="A63" s="4" t="s">
         <v>119</v>
       </c>
@@ -5199,7 +5206,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="15" customHeight="1">
       <c r="A64" s="4" t="s">
         <v>119</v>
       </c>
@@ -5213,7 +5220,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="15" customHeight="1">
       <c r="A65" s="4" t="s">
         <v>117</v>
       </c>
@@ -5227,7 +5234,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="15" customHeight="1">
       <c r="A66" s="4" t="s">
         <v>117</v>
       </c>
@@ -5241,7 +5248,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="15" customHeight="1">
       <c r="A67" s="4" t="s">
         <v>117</v>
       </c>
@@ -5255,7 +5262,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="15" customHeight="1">
       <c r="A68" s="4" t="s">
         <v>117</v>
       </c>
@@ -5269,7 +5276,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="15" customHeight="1">
       <c r="A69" s="4" t="s">
         <v>117</v>
       </c>
@@ -5283,7 +5290,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="15" customHeight="1">
       <c r="A70" s="4" t="s">
         <v>127</v>
       </c>
@@ -5297,7 +5304,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="15" customHeight="1">
       <c r="A71" s="4" t="s">
         <v>127</v>
       </c>
@@ -5311,7 +5318,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="15" customHeight="1">
       <c r="A72" s="4" t="s">
         <v>131</v>
       </c>
@@ -5325,7 +5332,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="15" customHeight="1">
       <c r="A73" s="4" t="s">
         <v>131</v>
       </c>
@@ -5339,7 +5346,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="15" customHeight="1">
       <c r="A74" s="4" t="s">
         <v>139</v>
       </c>
@@ -5353,7 +5360,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" ht="15" customHeight="1">
       <c r="A75" s="4" t="s">
         <v>139</v>
       </c>
@@ -5367,7 +5374,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" ht="15" customHeight="1">
       <c r="A76" s="4" t="s">
         <v>139</v>
       </c>
@@ -5381,7 +5388,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" ht="15" customHeight="1">
       <c r="A77" s="4" t="s">
         <v>139</v>
       </c>
@@ -5395,7 +5402,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="15" customHeight="1">
       <c r="A78" s="4" t="s">
         <v>139</v>
       </c>
@@ -5409,7 +5416,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" ht="15" customHeight="1">
       <c r="A79" s="4" t="s">
         <v>139</v>
       </c>
@@ -5423,7 +5430,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" ht="15" customHeight="1">
       <c r="A80" s="4" t="s">
         <v>137</v>
       </c>
@@ -5437,7 +5444,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" ht="15" customHeight="1">
       <c r="A81" s="4" t="s">
         <v>137</v>
       </c>
@@ -5451,7 +5458,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="15" customHeight="1">
       <c r="A82" s="4" t="s">
         <v>137</v>
       </c>
@@ -5465,7 +5472,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="15" customHeight="1">
       <c r="A83" s="4" t="s">
         <v>137</v>
       </c>
@@ -5479,7 +5486,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" ht="15" customHeight="1">
       <c r="A84" s="4" t="s">
         <v>137</v>
       </c>
@@ -5493,7 +5500,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" ht="15" customHeight="1">
       <c r="A85" s="4" t="s">
         <v>137</v>
       </c>
@@ -5507,7 +5514,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" ht="15" customHeight="1">
       <c r="A86" s="4" t="s">
         <v>137</v>
       </c>
@@ -5521,7 +5528,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" ht="15" customHeight="1">
       <c r="A87" s="4" t="s">
         <v>137</v>
       </c>
@@ -5535,7 +5542,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" ht="15" customHeight="1">
       <c r="A88" s="4" t="s">
         <v>147</v>
       </c>
@@ -5549,7 +5556,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" ht="15" customHeight="1">
       <c r="A89" s="4" t="s">
         <v>147</v>
       </c>
@@ -5563,7 +5570,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" ht="15" customHeight="1">
       <c r="A90" s="4" t="s">
         <v>151</v>
       </c>
@@ -5577,7 +5584,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" ht="15" customHeight="1">
       <c r="A91" s="4" t="s">
         <v>151</v>
       </c>
@@ -5591,7 +5598,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" ht="15" customHeight="1">
       <c r="A92" s="4" t="s">
         <v>159</v>
       </c>
@@ -5605,7 +5612,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" ht="15" customHeight="1">
       <c r="A93" s="4" t="s">
         <v>159</v>
       </c>
@@ -5619,7 +5626,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" ht="15" customHeight="1">
       <c r="A94" s="4" t="s">
         <v>159</v>
       </c>
@@ -5633,7 +5640,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" ht="15" customHeight="1">
       <c r="A95" s="4" t="s">
         <v>159</v>
       </c>
@@ -5647,7 +5654,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" ht="15" customHeight="1">
       <c r="A96" s="4" t="s">
         <v>159</v>
       </c>
@@ -5661,7 +5668,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" ht="15" customHeight="1">
       <c r="A97" s="4" t="s">
         <v>159</v>
       </c>
@@ -5675,7 +5682,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" ht="15" customHeight="1">
       <c r="A98" s="4" t="s">
         <v>157</v>
       </c>
@@ -5689,7 +5696,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="15" customHeight="1">
       <c r="A99" s="4" t="s">
         <v>157</v>
       </c>
@@ -5703,7 +5710,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" ht="15" customHeight="1">
       <c r="A100" s="4" t="s">
         <v>157</v>
       </c>
@@ -5717,7 +5724,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" ht="15" customHeight="1">
       <c r="A101" s="4" t="s">
         <v>157</v>
       </c>
@@ -5731,7 +5738,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" ht="15" customHeight="1">
       <c r="A102" s="4" t="s">
         <v>157</v>
       </c>
@@ -5745,7 +5752,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" ht="15" customHeight="1">
       <c r="A103" s="4" t="s">
         <v>157</v>
       </c>
@@ -5759,7 +5766,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" ht="15" customHeight="1">
       <c r="A104" s="4" t="s">
         <v>157</v>
       </c>
@@ -5773,7 +5780,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" ht="15" customHeight="1">
       <c r="A105" s="4" t="s">
         <v>157</v>
       </c>
@@ -5787,7 +5794,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" ht="15" customHeight="1">
       <c r="A106" s="4" t="s">
         <v>157</v>
       </c>
@@ -5801,7 +5808,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" ht="15" customHeight="1">
       <c r="A107" s="4" t="s">
         <v>157</v>
       </c>
@@ -5815,7 +5822,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" ht="15" customHeight="1">
       <c r="A108" s="4" t="s">
         <v>157</v>
       </c>
@@ -5829,7 +5836,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" ht="15" customHeight="1">
       <c r="A109" s="4" t="s">
         <v>157</v>
       </c>
@@ -5843,7 +5850,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" ht="15" customHeight="1">
       <c r="A110" s="4" t="s">
         <v>157</v>
       </c>
@@ -5857,7 +5864,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" ht="15" customHeight="1">
       <c r="A111" s="4" t="s">
         <v>157</v>
       </c>
@@ -5871,7 +5878,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" ht="15" customHeight="1">
       <c r="A112" s="4" t="s">
         <v>175</v>
       </c>
@@ -5885,7 +5892,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" ht="15" customHeight="1">
       <c r="A113" s="4" t="s">
         <v>175</v>
       </c>
@@ -5899,7 +5906,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" ht="15" customHeight="1">
       <c r="A114" s="4" t="s">
         <v>175</v>
       </c>
@@ -5913,7 +5920,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="15" customHeight="1">
       <c r="A115" s="4" t="s">
         <v>175</v>
       </c>
@@ -5927,7 +5934,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" ht="15" customHeight="1">
       <c r="A116" s="4" t="s">
         <v>175</v>
       </c>
@@ -5941,7 +5948,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" ht="15" customHeight="1">
       <c r="A117" s="4" t="s">
         <v>175</v>
       </c>
@@ -5955,7 +5962,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" ht="15" customHeight="1">
       <c r="A118" s="4" t="s">
         <v>173</v>
       </c>
@@ -5969,7 +5976,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" ht="15" customHeight="1">
       <c r="A119" s="4" t="s">
         <v>173</v>
       </c>
@@ -5983,7 +5990,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" ht="15" customHeight="1">
       <c r="A120" s="4" t="s">
         <v>173</v>
       </c>
@@ -5997,7 +6004,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" ht="15" customHeight="1">
       <c r="A121" s="4" t="s">
         <v>173</v>
       </c>
@@ -6011,7 +6018,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" ht="15" customHeight="1">
       <c r="A122" s="4" t="s">
         <v>173</v>
       </c>
@@ -6025,7 +6032,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" ht="15" customHeight="1">
       <c r="A123" s="4" t="s">
         <v>173</v>
       </c>
@@ -6039,7 +6046,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" ht="15" customHeight="1">
       <c r="A124" s="4" t="s">
         <v>173</v>
       </c>
@@ -6053,7 +6060,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" ht="15" customHeight="1">
       <c r="A125" s="4" t="s">
         <v>173</v>
       </c>
@@ -6067,7 +6074,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" ht="15" customHeight="1">
       <c r="A126" s="4" t="s">
         <v>173</v>
       </c>
@@ -6081,7 +6088,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" ht="15" customHeight="1">
       <c r="A127" s="4" t="s">
         <v>173</v>
       </c>
@@ -6095,7 +6102,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" ht="15" customHeight="1">
       <c r="A128" s="4" t="s">
         <v>173</v>
       </c>
@@ -6109,7 +6116,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" ht="15" customHeight="1">
       <c r="A129" s="4" t="s">
         <v>173</v>
       </c>
@@ -6123,7 +6130,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" ht="15" customHeight="1">
       <c r="A130" s="4" t="s">
         <v>173</v>
       </c>
@@ -6137,7 +6144,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" ht="15" customHeight="1">
       <c r="A131" s="4" t="s">
         <v>173</v>
       </c>
@@ -6151,7 +6158,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" ht="15" customHeight="1">
       <c r="A132" s="4" t="s">
         <v>173</v>
       </c>
@@ -6165,7 +6172,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" ht="15" customHeight="1">
       <c r="A133" s="4" t="s">
         <v>173</v>
       </c>
@@ -6179,7 +6186,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" ht="15" customHeight="1">
       <c r="A134" s="4" t="s">
         <v>173</v>
       </c>
@@ -6193,7 +6200,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" ht="15" customHeight="1">
       <c r="A135" s="4" t="s">
         <v>191</v>
       </c>
@@ -6207,7 +6214,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" ht="15" customHeight="1">
       <c r="A136" s="4" t="s">
         <v>191</v>
       </c>
@@ -6221,7 +6228,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" ht="15" customHeight="1">
       <c r="A137" s="4" t="s">
         <v>191</v>
       </c>
@@ -6235,7 +6242,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" ht="15" customHeight="1">
       <c r="A138" s="4" t="s">
         <v>191</v>
       </c>
@@ -6249,7 +6256,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" ht="15" customHeight="1">
       <c r="A139" s="4" t="s">
         <v>191</v>
       </c>
@@ -6263,7 +6270,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" ht="15" customHeight="1">
       <c r="A140" s="4" t="s">
         <v>191</v>
       </c>
@@ -6277,7 +6284,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" ht="15" customHeight="1">
       <c r="A141" s="4" t="s">
         <v>189</v>
       </c>
@@ -6291,7 +6298,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" ht="15" customHeight="1">
       <c r="A142" s="4" t="s">
         <v>189</v>
       </c>
@@ -6305,7 +6312,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" ht="15" customHeight="1">
       <c r="A143" s="4" t="s">
         <v>189</v>
       </c>
@@ -6319,7 +6326,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" ht="15" customHeight="1">
       <c r="A144" s="4" t="s">
         <v>189</v>
       </c>
@@ -6333,7 +6340,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" ht="15" customHeight="1">
       <c r="A145" s="4" t="s">
         <v>189</v>
       </c>
@@ -6347,7 +6354,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" ht="15" customHeight="1">
       <c r="A146" s="4" t="s">
         <v>189</v>
       </c>
@@ -6361,7 +6368,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" ht="15" customHeight="1">
       <c r="A147" s="4" t="s">
         <v>189</v>
       </c>
@@ -6375,7 +6382,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" ht="15" customHeight="1">
       <c r="A148" s="4" t="s">
         <v>189</v>
       </c>
@@ -6389,7 +6396,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" ht="15" customHeight="1">
       <c r="A149" s="4" t="s">
         <v>189</v>
       </c>
@@ -6403,7 +6410,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" ht="15" customHeight="1">
       <c r="A150" s="4" t="s">
         <v>189</v>
       </c>
@@ -6417,7 +6424,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" ht="15" customHeight="1">
       <c r="A151" s="4" t="s">
         <v>189</v>
       </c>
@@ -6431,7 +6438,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" ht="15" customHeight="1">
       <c r="A152" s="4" t="s">
         <v>189</v>
       </c>
@@ -6445,7 +6452,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" ht="15" customHeight="1">
       <c r="A153" s="4" t="s">
         <v>189</v>
       </c>
@@ -6459,7 +6466,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" ht="15" customHeight="1">
       <c r="A154" s="4" t="s">
         <v>189</v>
       </c>
@@ -6473,7 +6480,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" ht="15" customHeight="1">
       <c r="A155" s="4" t="s">
         <v>207</v>
       </c>
@@ -6487,7 +6494,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" ht="15" customHeight="1">
       <c r="A156" s="4" t="s">
         <v>207</v>
       </c>
@@ -6501,7 +6508,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" ht="15" customHeight="1">
       <c r="A157" s="4" t="s">
         <v>207</v>
       </c>
@@ -6515,7 +6522,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" ht="15" customHeight="1">
       <c r="A158" s="4" t="s">
         <v>207</v>
       </c>
@@ -6529,7 +6536,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" ht="15" customHeight="1">
       <c r="A159" s="4" t="s">
         <v>207</v>
       </c>
@@ -6543,7 +6550,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" ht="15" customHeight="1">
       <c r="A160" s="4" t="s">
         <v>207</v>
       </c>
@@ -6557,7 +6564,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" ht="15" customHeight="1">
       <c r="A161" s="4" t="s">
         <v>205</v>
       </c>
@@ -6571,7 +6578,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" ht="15" customHeight="1">
       <c r="A162" s="4" t="s">
         <v>205</v>
       </c>
@@ -6585,7 +6592,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" ht="15" customHeight="1">
       <c r="A163" s="4" t="s">
         <v>223</v>
       </c>
@@ -6599,7 +6606,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:4" ht="15" customHeight="1">
       <c r="A164" s="4" t="s">
         <v>223</v>
       </c>
@@ -6613,7 +6620,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:4" ht="15" customHeight="1">
       <c r="A165" s="4" t="s">
         <v>223</v>
       </c>
@@ -6627,7 +6634,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:4" ht="15" customHeight="1">
       <c r="A166" s="4" t="s">
         <v>223</v>
       </c>
@@ -6641,7 +6648,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:4" ht="15" customHeight="1">
       <c r="A167" s="4" t="s">
         <v>223</v>
       </c>
@@ -6655,7 +6662,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:4" ht="15" customHeight="1">
       <c r="A168" s="4" t="s">
         <v>223</v>
       </c>
@@ -6669,7 +6676,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:4" ht="15" customHeight="1">
       <c r="A169" s="4" t="s">
         <v>221</v>
       </c>
@@ -6683,7 +6690,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" ht="15" customHeight="1">
       <c r="A170" s="4" t="s">
         <v>221</v>
       </c>
@@ -6697,7 +6704,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:4" ht="15" customHeight="1">
       <c r="A171" s="4" t="s">
         <v>221</v>
       </c>
@@ -6711,7 +6718,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" ht="15" customHeight="1">
       <c r="A172" s="4" t="s">
         <v>221</v>
       </c>
@@ -6725,7 +6732,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:4" ht="15" customHeight="1">
       <c r="A173" s="4" t="s">
         <v>221</v>
       </c>
@@ -6739,7 +6746,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" ht="15" customHeight="1">
       <c r="A174" s="4" t="s">
         <v>221</v>
       </c>
@@ -6753,7 +6760,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" ht="15" customHeight="1">
       <c r="A175" s="4" t="s">
         <v>221</v>
       </c>
@@ -6767,7 +6774,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:4" ht="15" customHeight="1">
       <c r="A176" s="4" t="s">
         <v>221</v>
       </c>
@@ -6781,7 +6788,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" ht="15" customHeight="1">
       <c r="A177" s="4" t="s">
         <v>221</v>
       </c>
@@ -6795,7 +6802,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4" ht="15" customHeight="1">
       <c r="A178" s="4" t="s">
         <v>221</v>
       </c>
@@ -6809,7 +6816,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" ht="15" customHeight="1">
       <c r="A179" s="4" t="s">
         <v>221</v>
       </c>
@@ -6823,7 +6830,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" ht="15" customHeight="1">
       <c r="A180" s="4" t="s">
         <v>221</v>
       </c>
@@ -6837,7 +6844,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" ht="15" customHeight="1">
       <c r="A181" s="4" t="s">
         <v>221</v>
       </c>
@@ -6851,7 +6858,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" ht="15" customHeight="1">
       <c r="A182" s="4" t="s">
         <v>221</v>
       </c>
@@ -6865,7 +6872,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" ht="15" customHeight="1">
       <c r="A183" s="4" t="s">
         <v>221</v>
       </c>
@@ -6879,7 +6886,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:4" ht="15" customHeight="1">
       <c r="A184" s="4" t="s">
         <v>221</v>
       </c>
@@ -6893,7 +6900,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" ht="15" customHeight="1">
       <c r="A185" s="4" t="s">
         <v>221</v>
       </c>
@@ -6907,7 +6914,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" ht="15" customHeight="1">
       <c r="A186" s="4" t="s">
         <v>221</v>
       </c>
@@ -6921,7 +6928,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" ht="15" customHeight="1">
       <c r="A187" s="4" t="s">
         <v>221</v>
       </c>
@@ -6935,7 +6942,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:4" ht="15" customHeight="1">
       <c r="A188" s="4" t="s">
         <v>221</v>
       </c>
@@ -6949,7 +6956,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:4" ht="15" customHeight="1">
       <c r="A189" s="4" t="s">
         <v>221</v>
       </c>
@@ -6963,7 +6970,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:4" ht="15" customHeight="1">
       <c r="A190" s="4" t="s">
         <v>221</v>
       </c>
@@ -6977,7 +6984,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:4" ht="15" customHeight="1">
       <c r="A191" s="4" t="s">
         <v>221</v>
       </c>
@@ -6991,7 +6998,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:4" ht="15" customHeight="1">
       <c r="A192" s="4" t="s">
         <v>221</v>
       </c>
@@ -7005,7 +7012,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:4" ht="15" customHeight="1">
       <c r="A193" s="4" t="s">
         <v>221</v>
       </c>
@@ -7019,7 +7026,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:4" ht="15" customHeight="1">
       <c r="A194" s="4" t="s">
         <v>221</v>
       </c>
@@ -7033,7 +7040,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:4" ht="15" customHeight="1">
       <c r="A195" s="4" t="s">
         <v>221</v>
       </c>
@@ -7047,7 +7054,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:4" ht="15" customHeight="1">
       <c r="A196" s="4" t="s">
         <v>221</v>
       </c>
@@ -7061,7 +7068,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:4" ht="15" customHeight="1">
       <c r="A197" s="4" t="s">
         <v>221</v>
       </c>
@@ -7075,7 +7082,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:4" ht="15" customHeight="1">
       <c r="A198" s="8" t="s">
         <v>221</v>
       </c>
@@ -7089,7 +7096,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:4" ht="15" customHeight="1">
       <c r="A199" s="14" t="s">
         <v>303</v>
       </c>
@@ -7103,7 +7110,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:4" ht="15" customHeight="1">
       <c r="A200" s="14" t="s">
         <v>303</v>
       </c>
@@ -7117,7 +7124,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:4" ht="15" customHeight="1">
       <c r="A201" s="14" t="s">
         <v>305</v>
       </c>
@@ -7131,7 +7138,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:4" ht="15" customHeight="1">
       <c r="A202" s="14" t="s">
         <v>305</v>
       </c>
@@ -7145,7 +7152,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:4" ht="15" customHeight="1">
       <c r="A203" s="14" t="s">
         <v>307</v>
       </c>
@@ -7159,7 +7166,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:4" ht="15" customHeight="1">
       <c r="A204" s="14" t="s">
         <v>349</v>
       </c>
@@ -7173,7 +7180,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:4" ht="15" customHeight="1">
       <c r="A205" s="14" t="s">
         <v>309</v>
       </c>
@@ -7187,7 +7194,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:4" ht="15" customHeight="1">
       <c r="A206" s="14" t="s">
         <v>309</v>
       </c>
@@ -7201,7 +7208,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:4" ht="15" customHeight="1">
       <c r="A207" s="14" t="s">
         <v>311</v>
       </c>
@@ -7215,7 +7222,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:4" ht="15" customHeight="1">
       <c r="A208" s="14" t="s">
         <v>311</v>
       </c>
@@ -7229,7 +7236,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:4" ht="15" customHeight="1">
       <c r="A209" s="14" t="s">
         <v>313</v>
       </c>
@@ -7243,7 +7250,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:4" ht="15" customHeight="1">
       <c r="A210" s="14" t="s">
         <v>313</v>
       </c>
@@ -7257,7 +7264,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:4" ht="15" customHeight="1">
       <c r="A211" s="14" t="s">
         <v>315</v>
       </c>
@@ -7271,7 +7278,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:4" ht="15" customHeight="1">
       <c r="A212" s="14" t="s">
         <v>315</v>
       </c>
@@ -7285,7 +7292,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:4" ht="15" customHeight="1">
       <c r="A213" s="14" t="s">
         <v>317</v>
       </c>
@@ -7299,7 +7306,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:4" ht="15" customHeight="1">
       <c r="A214" s="14" t="s">
         <v>317</v>
       </c>
@@ -7313,7 +7320,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:4" ht="15" customHeight="1">
       <c r="A215" s="14" t="s">
         <v>319</v>
       </c>
@@ -7327,7 +7334,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:4" ht="15" customHeight="1">
       <c r="A216" s="14" t="s">
         <v>319</v>
       </c>
@@ -7341,7 +7348,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:4" ht="15" customHeight="1">
       <c r="A217" s="14" t="s">
         <v>321</v>
       </c>
@@ -7355,7 +7362,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:4" ht="15" customHeight="1">
       <c r="A218" s="14" t="s">
         <v>321</v>
       </c>
@@ -7369,7 +7376,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:4" ht="15" customHeight="1">
       <c r="A219" s="14" t="s">
         <v>323</v>
       </c>
@@ -7383,7 +7390,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:4" ht="15" customHeight="1">
       <c r="A220" s="14" t="s">
         <v>323</v>
       </c>
@@ -7397,7 +7404,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:4" ht="15" customHeight="1">
       <c r="A221" s="14" t="s">
         <v>325</v>
       </c>
@@ -7411,7 +7418,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:4" ht="15" customHeight="1">
       <c r="A222" s="14" t="s">
         <v>325</v>
       </c>
@@ -7425,7 +7432,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:4" ht="15" customHeight="1">
       <c r="A223" s="14" t="s">
         <v>327</v>
       </c>
@@ -7439,7 +7446,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:4" ht="15" customHeight="1">
       <c r="A224" s="14" t="s">
         <v>327</v>
       </c>
@@ -7453,7 +7460,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:4" ht="15" customHeight="1">
       <c r="A225" s="14" t="s">
         <v>329</v>
       </c>
@@ -7467,7 +7474,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:4" ht="15" customHeight="1">
       <c r="A226" s="14" t="s">
         <v>329</v>
       </c>
@@ -7481,7 +7488,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:4" ht="15" customHeight="1">
       <c r="A227" s="14" t="s">
         <v>331</v>
       </c>
@@ -7495,7 +7502,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="228" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:4" ht="15" customHeight="1">
       <c r="A228" s="14" t="s">
         <v>331</v>
       </c>
@@ -7509,7 +7516,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:4" ht="15" customHeight="1">
       <c r="A229" s="14" t="s">
         <v>333</v>
       </c>
@@ -7523,7 +7530,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="230" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:4" ht="15" customHeight="1">
       <c r="A230" s="14" t="s">
         <v>333</v>
       </c>
@@ -7537,7 +7544,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:4" ht="15" customHeight="1">
       <c r="A231" s="14" t="s">
         <v>335</v>
       </c>
@@ -7551,7 +7558,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:4" ht="15" customHeight="1">
       <c r="A232" s="14" t="s">
         <v>335</v>
       </c>
@@ -7565,7 +7572,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:4" ht="15" customHeight="1">
       <c r="A233" s="14" t="s">
         <v>337</v>
       </c>
@@ -7579,7 +7586,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:4" ht="15" customHeight="1">
       <c r="A234" s="14" t="s">
         <v>337</v>
       </c>
@@ -7593,7 +7600,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:4" ht="15" customHeight="1">
       <c r="A235" s="14" t="s">
         <v>339</v>
       </c>
@@ -7607,7 +7614,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="236" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:4" ht="15" customHeight="1">
       <c r="A236" s="14" t="s">
         <v>339</v>
       </c>
@@ -7621,7 +7628,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:4" ht="15" customHeight="1">
       <c r="A237" s="14" t="s">
         <v>341</v>
       </c>
@@ -7635,7 +7642,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:4" ht="15" customHeight="1">
       <c r="A238" s="14" t="s">
         <v>341</v>
       </c>
@@ -7649,7 +7656,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:4" ht="15" customHeight="1">
       <c r="A239" s="14" t="s">
         <v>343</v>
       </c>
@@ -7663,7 +7670,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:4" ht="15" customHeight="1">
       <c r="A240" s="14" t="s">
         <v>343</v>
       </c>
@@ -7677,7 +7684,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="241" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:4" ht="15" customHeight="1">
       <c r="A241" s="14" t="s">
         <v>345</v>
       </c>
@@ -7691,7 +7698,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="242" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:4" ht="15" customHeight="1">
       <c r="A242" s="14" t="s">
         <v>345</v>
       </c>
@@ -7705,7 +7712,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="243" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:4" ht="15" customHeight="1">
       <c r="A243" s="14" t="s">
         <v>347</v>
       </c>
@@ -7719,7 +7726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="244" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:4" ht="15" customHeight="1">
       <c r="A244" s="14" t="s">
         <v>347</v>
       </c>
@@ -7733,7 +7740,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="245" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:4" ht="15" customHeight="1">
       <c r="A245" s="20" t="s">
         <v>374</v>
       </c>
@@ -7747,7 +7754,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="246" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:4" ht="15" customHeight="1">
       <c r="A246" s="20" t="s">
         <v>374</v>
       </c>
@@ -7761,7 +7768,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="247" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:4" ht="15" customHeight="1">
       <c r="A247" s="20" t="s">
         <v>377</v>
       </c>
@@ -7775,7 +7782,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="248" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:4" ht="15" customHeight="1">
       <c r="A248" s="20" t="s">
         <v>377</v>
       </c>
@@ -7789,7 +7796,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="249" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:4" ht="15" customHeight="1">
       <c r="A249" s="20" t="s">
         <v>377</v>
       </c>
@@ -7803,7 +7810,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="250" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:4" ht="15" customHeight="1">
       <c r="A250" s="20" t="s">
         <v>381</v>
       </c>
@@ -7817,7 +7824,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="251" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:4" ht="15" customHeight="1">
       <c r="A251" s="20" t="s">
         <v>381</v>
       </c>
@@ -7831,7 +7838,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="252" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:4" ht="15" customHeight="1">
       <c r="A252" s="20" t="s">
         <v>381</v>
       </c>
@@ -7845,7 +7852,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="253" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:4" ht="15" customHeight="1">
       <c r="A253" s="20" t="s">
         <v>381</v>
       </c>
@@ -7859,7 +7866,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="254" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:4" ht="15" customHeight="1">
       <c r="A254" s="20" t="s">
         <v>381</v>
       </c>
@@ -7873,7 +7880,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="255" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:4" ht="15" customHeight="1">
       <c r="A255" s="20" t="s">
         <v>381</v>
       </c>
@@ -7887,7 +7894,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="256" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:4" ht="15" customHeight="1">
       <c r="A256" s="20" t="s">
         <v>381</v>
       </c>
@@ -7901,7 +7908,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="257" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:4" ht="15" customHeight="1">
       <c r="A257" s="20" t="s">
         <v>381</v>
       </c>
@@ -7915,7 +7922,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="258" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:4" ht="15" customHeight="1">
       <c r="A258" s="20" t="s">
         <v>381</v>
       </c>
@@ -7929,7 +7936,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="259" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:4" ht="15" customHeight="1">
       <c r="A259" s="20" t="s">
         <v>381</v>
       </c>
@@ -7943,7 +7950,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="260" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:4" ht="15" customHeight="1">
       <c r="A260" s="1" t="s">
         <v>395</v>
       </c>
@@ -7957,7 +7964,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="261" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:4" ht="15" customHeight="1">
       <c r="A261" s="1" t="s">
         <v>395</v>
       </c>
@@ -7971,7 +7978,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="262" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:4" ht="15" customHeight="1">
       <c r="A262" s="1" t="s">
         <v>399</v>
       </c>
@@ -7985,7 +7992,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="263" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:4" ht="15" customHeight="1">
       <c r="A263" s="1" t="s">
         <v>399</v>
       </c>
@@ -7999,7 +8006,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="264" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:4" ht="15" customHeight="1">
       <c r="A264" s="1" t="s">
         <v>403</v>
       </c>
@@ -8013,7 +8020,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="265" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:4" ht="15" customHeight="1">
       <c r="A265" s="1" t="s">
         <v>403</v>
       </c>
@@ -8027,7 +8034,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="266" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:4" ht="15" customHeight="1">
       <c r="A266" s="1" t="s">
         <v>407</v>
       </c>
@@ -8041,7 +8048,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="267" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:4" ht="15" customHeight="1">
       <c r="A267" s="1" t="s">
         <v>407</v>
       </c>
@@ -8055,7 +8062,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="268" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:4" ht="15" customHeight="1">
       <c r="A268" s="1" t="s">
         <v>411</v>
       </c>
@@ -8069,7 +8076,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="269" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:4" ht="15" customHeight="1">
       <c r="A269" s="1" t="s">
         <v>411</v>
       </c>
@@ -8083,7 +8090,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="270" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:4" ht="15" customHeight="1">
       <c r="A270" s="1" t="s">
         <v>415</v>
       </c>
@@ -8097,7 +8104,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="271" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:4" ht="15" customHeight="1">
       <c r="A271" s="1" t="s">
         <v>415</v>
       </c>
@@ -8111,7 +8118,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="272" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:4" ht="15" customHeight="1">
       <c r="A272" s="1" t="s">
         <v>419</v>
       </c>
@@ -8125,7 +8132,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:4" ht="15" customHeight="1">
       <c r="A273" s="1" t="s">
         <v>419</v>
       </c>
@@ -8139,7 +8146,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:4" ht="15" customHeight="1">
       <c r="A274" s="1" t="s">
         <v>423</v>
       </c>
@@ -8153,7 +8160,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="275" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:4" ht="15" customHeight="1">
       <c r="A275" s="1" t="s">
         <v>423</v>
       </c>
@@ -8167,7 +8174,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="276" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:4" ht="15" customHeight="1">
       <c r="A276" s="1" t="s">
         <v>427</v>
       </c>
@@ -8181,7 +8188,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="277" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:4" ht="15" customHeight="1">
       <c r="A277" s="1" t="s">
         <v>427</v>
       </c>
@@ -8195,7 +8202,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="278" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:4" ht="15" customHeight="1">
       <c r="A278" s="1" t="s">
         <v>431</v>
       </c>
@@ -8209,7 +8216,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="279" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:4" ht="15" customHeight="1">
       <c r="A279" s="1" t="s">
         <v>431</v>
       </c>

</xml_diff>

<commit_message>
adding sp_back in outcome yearly rep data
adding sp_back in outcome yearly rep data
</commit_message>
<xml_diff>
--- a/dictionaries/outcome/1_7/1_7_yearly_rep.xlsx
+++ b/dictionaries/outcome/1_7/1_7_yearly_rep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demetrisavraam/Desktop/GitHub/ds-dictionaries/dictionaries/outcome/1_7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA2AA96-F00B-AA4B-9ACA-190F2A91DF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB9EDD5-253A-4045-ABA8-EE094D5B4CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="443">
   <si>
     <t>name</t>
   </si>
@@ -1344,6 +1344,18 @@
   </si>
   <si>
     <t>high intensity</t>
+  </si>
+  <si>
+    <t>sp_back</t>
+  </si>
+  <si>
+    <t>Variable indicating whether the person has experienced any mid back or low back pain (combination of sp_midback and sp_lowback)</t>
+  </si>
+  <si>
+    <t>sp_back_age</t>
+  </si>
+  <si>
+    <t>Exact age of the child (in years) when spinal pain information was recorded for sp_back</t>
   </si>
 </sst>
 </file>
@@ -1991,10 +2003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG159"/>
+  <dimension ref="A1:BG161"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140:XFD159"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A160" sqref="A160:XFD161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4292,6 +4304,34 @@
         <v>434</v>
       </c>
     </row>
+    <row r="160" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="24" t="s">
+        <v>439</v>
+      </c>
+      <c r="B160" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C160" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D160" s="24" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="24" t="s">
+        <v>441</v>
+      </c>
+      <c r="B161" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C161" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D161" s="25" t="s">
+        <v>442</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
@@ -4304,10 +4344,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D279"/>
+  <dimension ref="A1:D281"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D238" sqref="D238"/>
+    <sheetView showGridLines="0" topLeftCell="A269" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A282" sqref="A282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8223,6 +8263,34 @@
         <v>438</v>
       </c>
     </row>
+    <row r="280" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A280" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="B280" s="1">
+        <v>0</v>
+      </c>
+      <c r="C280" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A281" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="B281" s="1">
+        <v>1</v>
+      </c>
+      <c r="C281" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="2048"/>

</xml_diff>